<commit_message>
update on ports and pins for ultrasonic, encoder, barcode
</commit_message>
<xml_diff>
--- a/Ports_Pins.xlsx
+++ b/Ports_Pins.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linwe\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SIT\CSC2003 Embedded Sys\git\robotic_Car\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C39A4347-CAA0-4151-80ED-3FA921ED36D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B1EE84-649C-441B-A9B2-42A7DAA07308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10200" xr2:uid="{A71EDA07-21D6-4961-9F6A-FABD12924A8F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A71EDA07-21D6-4961-9F6A-FABD12924A8F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Pins" sheetId="1" r:id="rId1"/>
+    <sheet name="Port Pins" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>Port</t>
   </si>
@@ -45,6 +45,30 @@
   </si>
   <si>
     <t>Sub-module</t>
+  </si>
+  <si>
+    <t>Encoder</t>
+  </si>
+  <si>
+    <t>GPIO Input (Interrupt)</t>
+  </si>
+  <si>
+    <t>Barcode Scanner</t>
+  </si>
+  <si>
+    <t>ADC Input</t>
+  </si>
+  <si>
+    <t>Ultrasonic</t>
+  </si>
+  <si>
+    <t>Trigger</t>
+  </si>
+  <si>
+    <t>Echo (Interrupt)</t>
+  </si>
+  <si>
+    <t>LED</t>
   </si>
 </sst>
 </file>
@@ -396,18 +420,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C849896-A32D-4B3B-8D61-CBF98F72A708}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -416,6 +441,90 @@
       </c>
       <c r="C1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>